<commit_message>
Data testing and design
</commit_message>
<xml_diff>
--- a/Design/TestData.xlsx
+++ b/Design/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nathanthomp\Programming\SportsBetter\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1344F6F9-D4C6-4DF3-8FB6-3530FB91BDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90633D9-FCC2-4D38-8BB6-46CC68C068FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24825" windowHeight="17490" xr2:uid="{3E0C60B0-723C-4EC8-A49E-AF8B637BBD37}"/>
+    <workbookView xWindow="21045" yWindow="675" windowWidth="24825" windowHeight="20085" xr2:uid="{3E0C60B0-723C-4EC8-A49E-AF8B637BBD37}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,101 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+  <si>
+    <t>TEN</t>
+  </si>
+  <si>
+    <t>CLE</t>
+  </si>
+  <si>
+    <t>DEN</t>
+  </si>
+  <si>
+    <t>MIA</t>
+  </si>
+  <si>
+    <t>BUF</t>
+  </si>
+  <si>
+    <t>WAS</t>
+  </si>
+  <si>
+    <t>HOU</t>
+  </si>
+  <si>
+    <t>JAX</t>
+  </si>
+  <si>
+    <t>ATL</t>
+  </si>
+  <si>
+    <t>DET</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>BAL</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>MIN</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NYJ</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>CAR</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>DAL</t>
+  </si>
+  <si>
+    <t>ARI</t>
+  </si>
+  <si>
+    <t>CHI</t>
+  </si>
+  <si>
+    <t>KC</t>
+  </si>
+  <si>
+    <t>PIT</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>PHI</t>
+  </si>
+  <si>
+    <t>TB</t>
+  </si>
+  <si>
+    <t>LAR</t>
+  </si>
+  <si>
+    <t>CIN</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,12 +477,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906067D0-CF7B-4C98-B9C4-6DD0C23C5DFB}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>-290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>-270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>-375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14">
+        <v>-170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>-395</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19">
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20">
+        <v>-112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>-148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25">
+        <v>-105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29">
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B35">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <v>-148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>26</v>
+      </c>
+      <c r="B40">
+        <v>-225</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B43">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>29</v>
+      </c>
+      <c r="B44">
+        <v>-162</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>